<commit_message>
add test suite files
</commit_message>
<xml_diff>
--- a/testSheet.xlsx
+++ b/testSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="120">
   <si>
     <t>Test no</t>
   </si>
@@ -378,6 +378,12 @@
   </si>
   <si>
     <t>Performance Testing</t>
+  </si>
+  <si>
+    <t>Notes and description</t>
+  </si>
+  <si>
+    <t>use typosaurus and other api's to check spelling mistakes</t>
   </si>
 </sst>
 </file>
@@ -739,10 +745,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I104"/>
+  <dimension ref="A1:J104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,7 +756,7 @@
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="162.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -759,7 +765,7 @@
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -770,25 +776,28 @@
         <v>86</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -798,8 +807,11 @@
       <c r="C2" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -810,7 +822,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -821,7 +833,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -832,7 +844,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -843,7 +855,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -854,7 +866,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -865,7 +877,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -876,7 +888,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -887,7 +899,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -898,7 +910,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -909,7 +921,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -920,7 +932,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -931,7 +943,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -942,7 +954,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>

</xml_diff>